<commit_message>
Big change: Shall be given a main_tone
</commit_message>
<xml_diff>
--- a/resources/scales/Midi_Notes.xlsx
+++ b/resources/scales/Midi_Notes.xlsx
@@ -1,35 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\creat\OneDrive\Fs\Harmony-Engines\resources\scales\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7284446-94C5-4678-9BB9-F97B8C0E05E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{026F9748-6AED-4917-BD32-4866A3067FBE}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -414,8 +394,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -426,10 +407,15 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -440,7 +426,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -452,29 +445,59 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+  <cellXfs count="15">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -485,10 +508,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -515,116 +538,82 @@
         <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -636,2131 +625,2161 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:tint val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:tint val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="9500"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot rev="0" lon="0" lat="0"/>
+            </a:camera>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:tint val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E573AA7-1BC6-4A1A-BEB6-0B5AE4253D27}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:E129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E129"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A2" s="5">
         <v>127</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="8">
         <v>12543.85</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A3" s="5">
         <v>126</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="8">
         <v>11839.82</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A4" s="5">
         <v>125</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="8">
         <v>11175.3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A5" s="5">
         <v>124</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="8">
         <v>10548.08</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A6" s="5">
         <v>123</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="8">
         <v>9956.06</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A7" s="5">
         <v>122</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="8">
         <v>9397.27</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A8" s="5">
         <v>121</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="8">
         <v>8869.84</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A9" s="5">
         <v>120</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="8">
         <v>8372.02</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A10" s="5">
         <v>119</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="8">
         <v>7902.13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A11" s="5">
         <v>118</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2" t="s">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="8">
         <v>7458.62</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="2">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A12" s="5">
         <v>117</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2" t="s">
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="5">
         <v>7040</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="2">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A13" s="5">
         <v>116</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2" t="s">
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="8">
         <v>6644.88</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="2">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A14" s="5">
         <v>115</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2" t="s">
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="8">
         <v>6271.93</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="2">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A15" s="5">
         <v>114</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2" t="s">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="8">
         <v>5919.91</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="2">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A16" s="5">
         <v>113</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2" t="s">
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="8">
         <v>5587.65</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="2">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A17" s="5">
         <v>112</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2" t="s">
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="8">
         <v>5274.04</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="2">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A18" s="5">
         <v>111</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2" t="s">
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="8">
         <v>4978.03</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="2">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A19" s="5">
         <v>110</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2" t="s">
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="2">
-        <v>4698.6400000000003</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="2">
+      <c r="E19" s="8">
+        <v>4698.64</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A20" s="5">
         <v>109</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2" t="s">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="8">
         <v>4434.92</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="2">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A21" s="5">
         <v>108</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2">
+      <c r="B21" s="6"/>
+      <c r="C21" s="5">
         <v>88</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="8">
         <v>4186.01</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="2">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A22" s="5">
         <v>107</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2">
+      <c r="B22" s="6"/>
+      <c r="C22" s="5">
         <v>87</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="8">
         <v>3951.07</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="2">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A23" s="5">
         <v>106</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2">
+      <c r="B23" s="6"/>
+      <c r="C23" s="5">
         <v>86</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="8">
         <v>3729.31</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="2">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A24" s="5">
         <v>105</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2">
+      <c r="B24" s="6"/>
+      <c r="C24" s="5">
         <v>85</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="5">
         <v>3520</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="2">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A25" s="5">
         <v>104</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2">
+      <c r="B25" s="6"/>
+      <c r="C25" s="5">
         <v>84</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="8">
         <v>3322.44</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="2">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A26" s="5">
         <v>103</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2">
+      <c r="B26" s="6"/>
+      <c r="C26" s="5">
         <v>83</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="8">
         <v>3135.96</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="2">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A27" s="5">
         <v>102</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2">
+      <c r="B27" s="6"/>
+      <c r="C27" s="5">
         <v>82</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="8">
         <v>2959.96</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="2">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A28" s="5">
         <v>101</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2">
+      <c r="B28" s="6"/>
+      <c r="C28" s="5">
         <v>81</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="8">
         <v>2793.83</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="2">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A29" s="5">
         <v>100</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2">
+      <c r="B29" s="6"/>
+      <c r="C29" s="5">
         <v>80</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="8">
         <v>2637.02</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="2">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A30" s="5">
         <v>99</v>
       </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2">
+      <c r="B30" s="6"/>
+      <c r="C30" s="5">
         <v>79</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="8">
         <v>2489.02</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="2">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A31" s="5">
         <v>98</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2">
+      <c r="B31" s="6"/>
+      <c r="C31" s="5">
         <v>78</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E31" s="2">
-        <v>2349.3200000000002</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="2">
+      <c r="E31" s="8">
+        <v>2349.32</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A32" s="5">
         <v>97</v>
       </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2">
+      <c r="B32" s="6"/>
+      <c r="C32" s="5">
         <v>77</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32" s="8">
         <v>2217.46</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="2">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A33" s="5">
         <v>96</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="5">
         <v>61</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="5">
         <v>76</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33" s="5">
         <v>2093</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="2">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A34" s="5">
         <v>95</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="5">
         <v>60</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="5">
         <v>75</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="8">
         <v>1975.53</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="2">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A35" s="5">
         <v>94</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35" s="5">
         <v>59</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="5">
         <v>74</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="8">
         <v>1864.66</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="2">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A36" s="5">
         <v>93</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36" s="5">
         <v>58</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="5">
         <v>73</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E36" s="5">
         <v>1760</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="2">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A37" s="5">
         <v>92</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37" s="5">
         <v>57</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="5">
         <v>72</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37" s="8">
         <v>1661.22</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="2">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A38" s="5">
         <v>91</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38" s="5">
         <v>56</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="5">
         <v>71</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38" s="8">
         <v>1567.98</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="2">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A39" s="5">
         <v>90</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39" s="5">
         <v>55</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="5">
         <v>70</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E39" s="8">
         <v>1479.98</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="2">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A40" s="5">
         <v>89</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40" s="5">
         <v>54</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="5">
         <v>69</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E40" s="2">
+      <c r="E40" s="8">
         <v>1396.91</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="2">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A41" s="5">
         <v>88</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41" s="5">
         <v>53</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="5">
         <v>68</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E41" s="8">
         <v>1318.51</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="2">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A42" s="5">
         <v>87</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42" s="5">
         <v>52</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="5">
         <v>67</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E42" s="8">
         <v>1244.51</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="2">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A43" s="5">
         <v>86</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43" s="5">
         <v>51</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="5">
         <v>66</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E43" s="2">
-        <v>1174.6600000000001</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="2">
+      <c r="E43" s="8">
+        <v>1174.66</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A44" s="5">
         <v>85</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44" s="5">
         <v>50</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="5">
         <v>65</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E44" s="2">
+      <c r="E44" s="8">
         <v>1108.73</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="2">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A45" s="5">
         <v>84</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="5">
         <v>49</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="5">
         <v>64</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E45" s="2">
+      <c r="E45" s="8">
         <v>1046.5</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="2">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A46" s="5">
         <v>83</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B46" s="5">
         <v>48</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="5">
         <v>63</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E46" s="2">
+      <c r="E46" s="8">
         <v>987.77</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="2">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A47" s="5">
         <v>82</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47" s="5">
         <v>47</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="5">
         <v>62</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E47" s="2">
+      <c r="E47" s="8">
         <v>932.33</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="2">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A48" s="5">
         <v>81</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48" s="5">
         <v>46</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="5">
         <v>61</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D48" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E48" s="2">
+      <c r="E48" s="5">
         <v>880</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="2">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A49" s="5">
         <v>80</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49" s="5">
         <v>45</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="5">
         <v>60</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D49" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E49" s="2">
+      <c r="E49" s="8">
         <v>830.61</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="2">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A50" s="5">
         <v>79</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B50" s="5">
         <v>44</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="5">
         <v>59</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D50" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E50" s="2">
+      <c r="E50" s="8">
         <v>783.99</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" s="2">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A51" s="5">
         <v>78</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51" s="5">
         <v>43</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51" s="5">
         <v>58</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D51" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E51" s="2">
+      <c r="E51" s="8">
         <v>739.99</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" s="2">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A52" s="5">
         <v>77</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B52" s="5">
         <v>42</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52" s="5">
         <v>57</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D52" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E52" s="2">
+      <c r="E52" s="8">
         <v>698.46</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A53" s="2">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A53" s="5">
         <v>76</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53" s="5">
         <v>41</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="5">
         <v>56</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D53" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E53" s="2">
+      <c r="E53" s="8">
         <v>659.26</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="2">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A54" s="5">
         <v>75</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B54" s="5">
         <v>40</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54" s="5">
         <v>55</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="D54" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E54" s="2">
+      <c r="E54" s="8">
         <v>622.25</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" s="2">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A55" s="5">
         <v>74</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B55" s="5">
         <v>39</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="5">
         <v>54</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D55" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E55" s="2">
-        <v>587.33000000000004</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" s="2">
+      <c r="E55" s="8">
+        <v>587.33</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A56" s="5">
         <v>73</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B56" s="5">
         <v>38</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56" s="5">
         <v>53</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D56" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E56" s="2">
+      <c r="E56" s="8">
         <v>554.37</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="2">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A57" s="5">
         <v>72</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B57" s="5">
         <v>37</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C57" s="5">
         <v>52</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="D57" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E57" s="2">
+      <c r="E57" s="8">
         <v>523.25</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" s="2">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A58" s="5">
         <v>71</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B58" s="5">
         <v>36</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C58" s="5">
         <v>51</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D58" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E58" s="2">
+      <c r="E58" s="8">
         <v>493.88</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" s="2">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A59" s="5">
         <v>70</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B59" s="5">
         <v>35</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C59" s="5">
         <v>50</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="D59" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E59" s="2">
+      <c r="E59" s="8">
         <v>466.16</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A60" s="2">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A60" s="5">
         <v>69</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B60" s="5">
         <v>34</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C60" s="5">
         <v>49</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D60" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E60" s="2">
+      <c r="E60" s="5">
         <v>440</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A61" s="2">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A61" s="5">
         <v>68</v>
       </c>
-      <c r="B61" s="2">
+      <c r="B61" s="5">
         <v>33</v>
       </c>
-      <c r="C61" s="2">
+      <c r="C61" s="5">
         <v>48</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="D61" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E61" s="2">
+      <c r="E61" s="8">
         <v>415.3</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" s="2">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A62" s="5">
         <v>67</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B62" s="5">
         <v>32</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62" s="5">
         <v>47</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="D62" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E62" s="2">
+      <c r="E62" s="5">
         <v>392</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A63" s="2">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A63" s="5">
         <v>66</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B63" s="5">
         <v>31</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C63" s="5">
         <v>46</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="D63" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E63" s="2">
+      <c r="E63" s="8">
         <v>369.99</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64" s="2">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A64" s="5">
         <v>65</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B64" s="5">
         <v>30</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C64" s="5">
         <v>45</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="D64" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E64" s="2">
+      <c r="E64" s="8">
         <v>349.23</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A65" s="2">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A65" s="5">
         <v>64</v>
       </c>
-      <c r="B65" s="2">
+      <c r="B65" s="5">
         <v>29</v>
       </c>
-      <c r="C65" s="2">
+      <c r="C65" s="5">
         <v>44</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="D65" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E65" s="2">
+      <c r="E65" s="8">
         <v>329.63</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A66" s="2">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A66" s="5">
         <v>63</v>
       </c>
-      <c r="B66" s="2">
+      <c r="B66" s="5">
         <v>28</v>
       </c>
-      <c r="C66" s="2">
+      <c r="C66" s="5">
         <v>43</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="D66" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E66" s="2">
+      <c r="E66" s="8">
         <v>311.13</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A67" s="2">
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A67" s="5">
         <v>62</v>
       </c>
-      <c r="B67" s="2">
+      <c r="B67" s="5">
         <v>27</v>
       </c>
-      <c r="C67" s="2">
+      <c r="C67" s="5">
         <v>42</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D67" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="E67" s="2">
-        <v>293.66000000000003</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A68" s="2">
+      <c r="E67" s="8">
+        <v>293.66</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A68" s="5">
         <v>61</v>
       </c>
-      <c r="B68" s="2">
+      <c r="B68" s="5">
         <v>26</v>
       </c>
-      <c r="C68" s="2">
+      <c r="C68" s="5">
         <v>41</v>
       </c>
-      <c r="D68" s="2" t="s">
+      <c r="D68" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E68" s="2">
+      <c r="E68" s="8">
         <v>277.18</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A69" s="3">
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A69" s="9">
         <v>60</v>
       </c>
-      <c r="B69" s="2">
+      <c r="B69" s="5">
         <v>25</v>
       </c>
-      <c r="C69" s="2">
+      <c r="C69" s="5">
         <v>40</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="D69" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E69" s="2">
+      <c r="E69" s="8">
         <v>261.63</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A70" s="2">
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A70" s="5">
         <v>59</v>
       </c>
-      <c r="B70" s="2">
+      <c r="B70" s="5">
         <v>24</v>
       </c>
-      <c r="C70" s="2">
+      <c r="C70" s="5">
         <v>39</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="D70" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E70" s="2">
+      <c r="E70" s="8">
         <v>246.94</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A71" s="2">
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A71" s="5">
         <v>58</v>
       </c>
-      <c r="B71" s="2">
+      <c r="B71" s="5">
         <v>23</v>
       </c>
-      <c r="C71" s="2">
+      <c r="C71" s="5">
         <v>38</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D71" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E71" s="2">
+      <c r="E71" s="8">
         <v>233.08</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A72" s="2">
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A72" s="5">
         <v>57</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B72" s="5">
         <v>22</v>
       </c>
-      <c r="C72" s="2">
+      <c r="C72" s="5">
         <v>37</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="D72" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E72" s="2">
+      <c r="E72" s="5">
         <v>220</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A73" s="2">
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A73" s="5">
         <v>56</v>
       </c>
-      <c r="B73" s="2">
+      <c r="B73" s="5">
         <v>21</v>
       </c>
-      <c r="C73" s="2">
+      <c r="C73" s="5">
         <v>36</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="D73" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="E73" s="2">
+      <c r="E73" s="8">
         <v>207.65</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A74" s="2">
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A74" s="5">
         <v>55</v>
       </c>
-      <c r="B74" s="2">
+      <c r="B74" s="5">
         <v>20</v>
       </c>
-      <c r="C74" s="2">
+      <c r="C74" s="5">
         <v>35</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="D74" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E74" s="2">
+      <c r="E74" s="5">
         <v>196</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A75" s="2">
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A75" s="5">
         <v>54</v>
       </c>
-      <c r="B75" s="2">
+      <c r="B75" s="5">
         <v>19</v>
       </c>
-      <c r="C75" s="2">
+      <c r="C75" s="5">
         <v>34</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="D75" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E75" s="2">
+      <c r="E75" s="5">
         <v>185</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A76" s="2">
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A76" s="5">
         <v>53</v>
       </c>
-      <c r="B76" s="2">
+      <c r="B76" s="5">
         <v>18</v>
       </c>
-      <c r="C76" s="2">
+      <c r="C76" s="5">
         <v>33</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="D76" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E76" s="2">
+      <c r="E76" s="8">
         <v>174.61</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A77" s="2">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A77" s="5">
         <v>52</v>
       </c>
-      <c r="B77" s="2">
+      <c r="B77" s="5">
         <v>17</v>
       </c>
-      <c r="C77" s="2">
+      <c r="C77" s="5">
         <v>32</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="D77" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="E77" s="2">
+      <c r="E77" s="8">
         <v>164.81</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A78" s="2">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A78" s="5">
         <v>51</v>
       </c>
-      <c r="B78" s="2">
+      <c r="B78" s="5">
         <v>16</v>
       </c>
-      <c r="C78" s="2">
+      <c r="C78" s="5">
         <v>31</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="D78" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E78" s="2">
+      <c r="E78" s="8">
         <v>155.56</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A79" s="2">
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A79" s="5">
         <v>50</v>
       </c>
-      <c r="B79" s="2">
+      <c r="B79" s="5">
         <v>15</v>
       </c>
-      <c r="C79" s="2">
+      <c r="C79" s="5">
         <v>30</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="D79" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E79" s="2">
-        <v>146.83000000000001</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A80" s="2">
+      <c r="E79" s="8">
+        <v>146.83</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A80" s="5">
         <v>49</v>
       </c>
-      <c r="B80" s="2">
+      <c r="B80" s="5">
         <v>14</v>
       </c>
-      <c r="C80" s="2">
+      <c r="C80" s="5">
         <v>29</v>
       </c>
-      <c r="D80" s="2" t="s">
+      <c r="D80" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E80" s="2">
+      <c r="E80" s="8">
         <v>138.59</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A81" s="2">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A81" s="5">
         <v>48</v>
       </c>
-      <c r="B81" s="2">
+      <c r="B81" s="5">
         <v>13</v>
       </c>
-      <c r="C81" s="2">
+      <c r="C81" s="5">
         <v>28</v>
       </c>
-      <c r="D81" s="2" t="s">
+      <c r="D81" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E81" s="2">
+      <c r="E81" s="8">
         <v>130.81</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A82" s="2">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A82" s="5">
         <v>47</v>
       </c>
-      <c r="B82" s="2">
+      <c r="B82" s="5">
         <v>12</v>
       </c>
-      <c r="C82" s="2">
+      <c r="C82" s="5">
         <v>27</v>
       </c>
-      <c r="D82" s="2" t="s">
+      <c r="D82" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="E82" s="2">
+      <c r="E82" s="8">
         <v>123.47</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A83" s="2">
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A83" s="5">
         <v>46</v>
       </c>
-      <c r="B83" s="2">
+      <c r="B83" s="5">
         <v>11</v>
       </c>
-      <c r="C83" s="2">
+      <c r="C83" s="5">
         <v>26</v>
       </c>
-      <c r="D83" s="2" t="s">
+      <c r="D83" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E83" s="2">
+      <c r="E83" s="8">
         <v>116.54</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A84" s="2">
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A84" s="5">
         <v>45</v>
       </c>
-      <c r="B84" s="2">
+      <c r="B84" s="5">
         <v>10</v>
       </c>
-      <c r="C84" s="2">
+      <c r="C84" s="5">
         <v>25</v>
       </c>
-      <c r="D84" s="2" t="s">
+      <c r="D84" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E84" s="2">
+      <c r="E84" s="5">
         <v>110</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A85" s="2">
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A85" s="5">
         <v>44</v>
       </c>
-      <c r="B85" s="2">
+      <c r="B85" s="5">
         <v>9</v>
       </c>
-      <c r="C85" s="2">
+      <c r="C85" s="5">
         <v>24</v>
       </c>
-      <c r="D85" s="2" t="s">
+      <c r="D85" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E85" s="2">
+      <c r="E85" s="8">
         <v>103.83</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A86" s="2">
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A86" s="5">
         <v>43</v>
       </c>
-      <c r="B86" s="2">
+      <c r="B86" s="5">
         <v>8</v>
       </c>
-      <c r="C86" s="2">
+      <c r="C86" s="5">
         <v>23</v>
       </c>
-      <c r="D86" s="2" t="s">
+      <c r="D86" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E86" s="2">
+      <c r="E86" s="5">
         <v>98</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A87" s="2">
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A87" s="5">
         <v>42</v>
       </c>
-      <c r="B87" s="2">
+      <c r="B87" s="5">
         <v>7</v>
       </c>
-      <c r="C87" s="2">
+      <c r="C87" s="5">
         <v>22</v>
       </c>
-      <c r="D87" s="2" t="s">
+      <c r="D87" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E87" s="2">
+      <c r="E87" s="8">
         <v>92.5</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A88" s="2">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A88" s="5">
         <v>41</v>
       </c>
-      <c r="B88" s="2">
+      <c r="B88" s="5">
         <v>6</v>
       </c>
-      <c r="C88" s="2">
+      <c r="C88" s="5">
         <v>21</v>
       </c>
-      <c r="D88" s="2" t="s">
+      <c r="D88" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="E88" s="2">
+      <c r="E88" s="8">
         <v>87.31</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A89" s="2">
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A89" s="5">
         <v>40</v>
       </c>
-      <c r="B89" s="2">
+      <c r="B89" s="5">
         <v>5</v>
       </c>
-      <c r="C89" s="2">
+      <c r="C89" s="5">
         <v>20</v>
       </c>
-      <c r="D89" s="2" t="s">
+      <c r="D89" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="E89" s="2">
+      <c r="E89" s="8">
         <v>82.41</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A90" s="2">
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A90" s="5">
         <v>39</v>
       </c>
-      <c r="B90" s="2">
+      <c r="B90" s="5">
         <v>4</v>
       </c>
-      <c r="C90" s="2">
+      <c r="C90" s="5">
         <v>19</v>
       </c>
-      <c r="D90" s="2" t="s">
+      <c r="D90" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="E90" s="2">
+      <c r="E90" s="8">
         <v>77.78</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A91" s="2">
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A91" s="5">
         <v>38</v>
       </c>
-      <c r="B91" s="2">
+      <c r="B91" s="5">
         <v>3</v>
       </c>
-      <c r="C91" s="2">
+      <c r="C91" s="5">
         <v>18</v>
       </c>
-      <c r="D91" s="2" t="s">
+      <c r="D91" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="E91" s="2">
+      <c r="E91" s="8">
         <v>73.42</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A92" s="2">
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A92" s="5">
         <v>37</v>
       </c>
-      <c r="B92" s="2">
+      <c r="B92" s="5">
         <v>2</v>
       </c>
-      <c r="C92" s="2">
+      <c r="C92" s="5">
         <v>17</v>
       </c>
-      <c r="D92" s="2" t="s">
+      <c r="D92" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E92" s="2">
+      <c r="E92" s="8">
         <v>69.3</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A93" s="2">
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A93" s="5">
         <v>36</v>
       </c>
-      <c r="B93" s="2">
+      <c r="B93" s="5">
         <v>1</v>
       </c>
-      <c r="C93" s="2">
+      <c r="C93" s="5">
         <v>16</v>
       </c>
-      <c r="D93" s="2" t="s">
+      <c r="D93" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="E93" s="2">
+      <c r="E93" s="8">
         <v>65.41</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A94" s="2">
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A94" s="5">
         <v>35</v>
       </c>
-      <c r="B94" s="2"/>
-      <c r="C94" s="2">
+      <c r="B94" s="6"/>
+      <c r="C94" s="5">
         <v>15</v>
       </c>
-      <c r="D94" s="2" t="s">
+      <c r="D94" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E94" s="2">
+      <c r="E94" s="8">
         <v>61.74</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A95" s="2">
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A95" s="5">
         <v>34</v>
       </c>
-      <c r="B95" s="2"/>
-      <c r="C95" s="2">
+      <c r="B95" s="6"/>
+      <c r="C95" s="5">
         <v>14</v>
       </c>
-      <c r="D95" s="2" t="s">
+      <c r="D95" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E95" s="2">
+      <c r="E95" s="8">
         <v>58.27</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A96" s="2">
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A96" s="5">
         <v>33</v>
       </c>
-      <c r="B96" s="2"/>
-      <c r="C96" s="2">
+      <c r="B96" s="6"/>
+      <c r="C96" s="5">
         <v>13</v>
       </c>
-      <c r="D96" s="2" t="s">
+      <c r="D96" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E96" s="2">
+      <c r="E96" s="5">
         <v>55</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A97" s="2">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A97" s="5">
         <v>32</v>
       </c>
-      <c r="B97" s="2"/>
-      <c r="C97" s="2">
+      <c r="B97" s="6"/>
+      <c r="C97" s="5">
         <v>12</v>
       </c>
-      <c r="D97" s="2" t="s">
+      <c r="D97" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="E97" s="2">
+      <c r="E97" s="8">
         <v>51.91</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A98" s="2">
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A98" s="5">
         <v>31</v>
       </c>
-      <c r="B98" s="2"/>
-      <c r="C98" s="2">
+      <c r="B98" s="6"/>
+      <c r="C98" s="5">
         <v>11</v>
       </c>
-      <c r="D98" s="2" t="s">
+      <c r="D98" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E98" s="2">
+      <c r="E98" s="5">
         <v>49</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A99" s="2">
+    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A99" s="5">
         <v>30</v>
       </c>
-      <c r="B99" s="2"/>
-      <c r="C99" s="2">
+      <c r="B99" s="6"/>
+      <c r="C99" s="5">
         <v>10</v>
       </c>
-      <c r="D99" s="2" t="s">
+      <c r="D99" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E99" s="2">
+      <c r="E99" s="8">
         <v>46.25</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A100" s="2">
+    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A100" s="5">
         <v>29</v>
       </c>
-      <c r="B100" s="2"/>
-      <c r="C100" s="2">
+      <c r="B100" s="6"/>
+      <c r="C100" s="5">
         <v>9</v>
       </c>
-      <c r="D100" s="2" t="s">
+      <c r="D100" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E100" s="2">
+      <c r="E100" s="8">
         <v>43.65</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A101" s="2">
+    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A101" s="5">
         <v>28</v>
       </c>
-      <c r="B101" s="2"/>
-      <c r="C101" s="2">
+      <c r="B101" s="6"/>
+      <c r="C101" s="5">
         <v>8</v>
       </c>
-      <c r="D101" s="2" t="s">
+      <c r="D101" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E101" s="2">
+      <c r="E101" s="8">
         <v>41.2</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A102" s="2">
+    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A102" s="5">
         <v>27</v>
       </c>
-      <c r="B102" s="2"/>
-      <c r="C102" s="2">
+      <c r="B102" s="6"/>
+      <c r="C102" s="5">
         <v>7</v>
       </c>
-      <c r="D102" s="2" t="s">
+      <c r="D102" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="E102" s="2">
+      <c r="E102" s="8">
         <v>38.89</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A103" s="2">
+    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A103" s="5">
         <v>26</v>
       </c>
-      <c r="B103" s="2"/>
-      <c r="C103" s="2">
+      <c r="B103" s="6"/>
+      <c r="C103" s="5">
         <v>6</v>
       </c>
-      <c r="D103" s="2" t="s">
+      <c r="D103" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E103" s="2">
+      <c r="E103" s="8">
         <v>36.71</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A104" s="2">
+    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A104" s="5">
         <v>25</v>
       </c>
-      <c r="B104" s="2"/>
-      <c r="C104" s="2">
+      <c r="B104" s="6"/>
+      <c r="C104" s="5">
         <v>5</v>
       </c>
-      <c r="D104" s="2" t="s">
+      <c r="D104" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="E104" s="2">
+      <c r="E104" s="8">
         <v>34.65</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A105" s="2">
+    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A105" s="5">
         <v>24</v>
       </c>
-      <c r="B105" s="2"/>
-      <c r="C105" s="2">
+      <c r="B105" s="6"/>
+      <c r="C105" s="5">
         <v>4</v>
       </c>
-      <c r="D105" s="2" t="s">
+      <c r="D105" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E105" s="2">
-        <v>32.700000000000003</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A106" s="2">
+      <c r="E105" s="8">
+        <v>32.7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A106" s="5">
         <v>23</v>
       </c>
-      <c r="B106" s="2"/>
-      <c r="C106" s="2">
+      <c r="B106" s="6"/>
+      <c r="C106" s="5">
         <v>3</v>
       </c>
-      <c r="D106" s="2" t="s">
+      <c r="D106" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="E106" s="2">
+      <c r="E106" s="8">
         <v>30.87</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A107" s="2">
+    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A107" s="5">
         <v>22</v>
       </c>
-      <c r="B107" s="2"/>
-      <c r="C107" s="2">
+      <c r="B107" s="6"/>
+      <c r="C107" s="5">
         <v>2</v>
       </c>
-      <c r="D107" s="2" t="s">
+      <c r="D107" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="E107" s="2">
+      <c r="E107" s="8">
         <v>29.14</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A108" s="2">
+    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A108" s="5">
         <v>21</v>
       </c>
-      <c r="B108" s="2"/>
-      <c r="C108" s="2">
+      <c r="B108" s="6"/>
+      <c r="C108" s="5">
         <v>1</v>
       </c>
-      <c r="D108" s="2" t="s">
+      <c r="D108" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="E108" s="2">
+      <c r="E108" s="8">
         <v>27.5</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A109" s="2">
+    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A109" s="5">
         <v>20</v>
       </c>
-      <c r="B109" s="2"/>
-      <c r="C109" s="2"/>
-      <c r="D109" s="2" t="s">
+      <c r="B109" s="6"/>
+      <c r="C109" s="6"/>
+      <c r="D109" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="E109" s="2">
+      <c r="E109" s="8">
         <v>25.96</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A110" s="2">
+    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A110" s="5">
         <v>19</v>
       </c>
-      <c r="B110" s="2"/>
-      <c r="C110" s="2"/>
-      <c r="D110" s="2" t="s">
+      <c r="B110" s="6"/>
+      <c r="C110" s="6"/>
+      <c r="D110" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="E110" s="2">
+      <c r="E110" s="8">
         <v>24.5</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A111" s="2">
+    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A111" s="5">
         <v>18</v>
       </c>
-      <c r="B111" s="2"/>
-      <c r="C111" s="2"/>
-      <c r="D111" s="2" t="s">
+      <c r="B111" s="6"/>
+      <c r="C111" s="6"/>
+      <c r="D111" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="E111" s="2">
+      <c r="E111" s="8">
         <v>23.12</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A112" s="2">
+    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A112" s="5">
         <v>17</v>
       </c>
-      <c r="B112" s="2"/>
-      <c r="C112" s="2"/>
-      <c r="D112" s="2" t="s">
+      <c r="B112" s="6"/>
+      <c r="C112" s="6"/>
+      <c r="D112" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="E112" s="2">
+      <c r="E112" s="8">
         <v>21.83</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A113" s="2">
+    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A113" s="5">
         <v>16</v>
       </c>
-      <c r="B113" s="2"/>
-      <c r="C113" s="2"/>
-      <c r="D113" s="2" t="s">
+      <c r="B113" s="6"/>
+      <c r="C113" s="6"/>
+      <c r="D113" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="E113" s="2">
+      <c r="E113" s="8">
         <v>20.6</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A114" s="2">
+    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A114" s="5">
         <v>15</v>
       </c>
-      <c r="B114" s="2"/>
-      <c r="C114" s="2"/>
-      <c r="D114" s="2" t="s">
+      <c r="B114" s="6"/>
+      <c r="C114" s="6"/>
+      <c r="D114" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="E114" s="2">
+      <c r="E114" s="8">
         <v>19.45</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A115" s="2">
+    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A115" s="5">
         <v>14</v>
       </c>
-      <c r="B115" s="2"/>
-      <c r="C115" s="2"/>
-      <c r="D115" s="2" t="s">
+      <c r="B115" s="6"/>
+      <c r="C115" s="6"/>
+      <c r="D115" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="E115" s="2">
-        <v>18.350000000000001</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A116" s="2">
+      <c r="E115" s="8">
+        <v>18.35</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A116" s="5">
         <v>13</v>
       </c>
-      <c r="B116" s="2"/>
-      <c r="C116" s="2"/>
-      <c r="D116" s="2" t="s">
+      <c r="B116" s="6"/>
+      <c r="C116" s="6"/>
+      <c r="D116" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="E116" s="2">
+      <c r="E116" s="8">
         <v>17.32</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A117" s="2">
+    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A117" s="5">
         <v>12</v>
       </c>
-      <c r="B117" s="2"/>
-      <c r="C117" s="2"/>
-      <c r="D117" s="2" t="s">
+      <c r="B117" s="6"/>
+      <c r="C117" s="6"/>
+      <c r="D117" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="E117" s="2">
-        <v>16.350000000000001</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A118" s="2">
+      <c r="E117" s="8">
+        <v>16.35</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A118" s="5">
         <v>11</v>
       </c>
-      <c r="B118" s="2"/>
-      <c r="C118" s="2"/>
-      <c r="D118" s="2" t="s">
+      <c r="B118" s="6"/>
+      <c r="C118" s="6"/>
+      <c r="D118" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="E118" s="2">
+      <c r="E118" s="8">
         <v>15.43</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A119" s="2">
+    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A119" s="5">
         <v>10</v>
       </c>
-      <c r="B119" s="2"/>
-      <c r="C119" s="2"/>
-      <c r="D119" s="2" t="s">
+      <c r="B119" s="6"/>
+      <c r="C119" s="6"/>
+      <c r="D119" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="E119" s="2">
+      <c r="E119" s="8">
         <v>14.57</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A120" s="2">
+    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A120" s="5">
         <v>9</v>
       </c>
-      <c r="B120" s="2"/>
-      <c r="C120" s="2"/>
-      <c r="D120" s="2" t="s">
+      <c r="B120" s="6"/>
+      <c r="C120" s="6"/>
+      <c r="D120" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="E120" s="2">
+      <c r="E120" s="8">
         <v>13.75</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A121" s="2">
+    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A121" s="5">
         <v>8</v>
       </c>
-      <c r="B121" s="2"/>
-      <c r="C121" s="2"/>
-      <c r="D121" s="2" t="s">
+      <c r="B121" s="6"/>
+      <c r="C121" s="6"/>
+      <c r="D121" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="E121" s="2">
+      <c r="E121" s="8">
         <v>12.98</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A122" s="2">
+    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A122" s="5">
         <v>7</v>
       </c>
-      <c r="B122" s="2"/>
-      <c r="C122" s="2"/>
-      <c r="D122" s="2" t="s">
+      <c r="B122" s="6"/>
+      <c r="C122" s="6"/>
+      <c r="D122" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="E122" s="2">
+      <c r="E122" s="8">
         <v>12.25</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A123" s="2">
+    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A123" s="5">
         <v>6</v>
       </c>
-      <c r="B123" s="2"/>
-      <c r="C123" s="2"/>
-      <c r="D123" s="2" t="s">
+      <c r="B123" s="6"/>
+      <c r="C123" s="6"/>
+      <c r="D123" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="E123" s="2">
+      <c r="E123" s="8">
         <v>11.56</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A124" s="2">
+    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A124" s="5">
         <v>5</v>
       </c>
-      <c r="B124" s="2"/>
-      <c r="C124" s="2"/>
-      <c r="D124" s="2" t="s">
+      <c r="B124" s="6"/>
+      <c r="C124" s="6"/>
+      <c r="D124" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="E124" s="2">
+      <c r="E124" s="8">
         <v>10.91</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A125" s="2">
+    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A125" s="5">
         <v>4</v>
       </c>
-      <c r="B125" s="2"/>
-      <c r="C125" s="2"/>
-      <c r="D125" s="2" t="s">
+      <c r="B125" s="6"/>
+      <c r="C125" s="6"/>
+      <c r="D125" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="E125" s="2">
+      <c r="E125" s="8">
         <v>10.3</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A126" s="2">
+    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A126" s="5">
         <v>3</v>
       </c>
-      <c r="B126" s="2"/>
-      <c r="C126" s="2"/>
-      <c r="D126" s="2" t="s">
+      <c r="B126" s="6"/>
+      <c r="C126" s="6"/>
+      <c r="D126" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="E126" s="2">
-        <v>9.7200000000000006</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A127" s="2">
+      <c r="E126" s="8">
+        <v>9.72</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A127" s="5">
         <v>2</v>
       </c>
-      <c r="B127" s="2"/>
-      <c r="C127" s="2"/>
-      <c r="D127" s="2" t="s">
+      <c r="B127" s="6"/>
+      <c r="C127" s="6"/>
+      <c r="D127" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="E127" s="2">
+      <c r="E127" s="8">
         <v>9.18</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A128" s="2">
+    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A128" s="5">
         <v>1</v>
       </c>
-      <c r="B128" s="2"/>
-      <c r="C128" s="2"/>
-      <c r="D128" s="2" t="s">
+      <c r="B128" s="6"/>
+      <c r="C128" s="6"/>
+      <c r="D128" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="E128" s="2">
+      <c r="E128" s="8">
         <v>8.66</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A129" s="2">
+    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A129" s="5">
         <v>0</v>
       </c>
-      <c r="B129" s="2"/>
-      <c r="C129" s="2"/>
-      <c r="D129" s="2" t="s">
+      <c r="B129" s="6"/>
+      <c r="C129" s="6"/>
+      <c r="D129" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="E129" s="2">
+      <c r="E129" s="8">
         <v>8.18</v>
       </c>
     </row>

</xml_diff>